<commit_message>
worked on java oops
</commit_message>
<xml_diff>
--- a/Data_Visualization/Day1/Practise.xlsx
+++ b/Data_Visualization/Day1/Practise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CDAC_Course\Data_Visualization\Day1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5589FD22-9A03-477C-967D-7EE4E112CF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE37BDE0-DC25-48A1-8A18-A3D6EE2236B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Actual Profit</t>
   </si>
@@ -52,18 +52,6 @@
   </si>
   <si>
     <t>Marketing</t>
-  </si>
-  <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Actual</t>
   </si>
 </sst>
 </file>
@@ -480,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,7 +483,7 @@
     <col min="6" max="6" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,11 +502,9 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>94</v>
       </c>
@@ -537,15 +523,8 @@
       <c r="F2" s="4">
         <v>24</v>
       </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2">
-        <f>MAX(A2:A31)</f>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>68</v>
       </c>
@@ -564,15 +543,8 @@
       <c r="F3" s="6">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3">
-        <f>MIN(A2:A31)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>101</v>
       </c>
@@ -592,7 +564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>30</v>
       </c>
@@ -611,15 +583,8 @@
       <c r="F5" s="6">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <f>I2-I3</f>
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>54</v>
       </c>
@@ -639,7 +604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>53</v>
       </c>
@@ -659,7 +624,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>99</v>
       </c>
@@ -679,7 +644,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>0</v>
       </c>
@@ -699,7 +664,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>33</v>
       </c>
@@ -719,7 +684,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>17</v>
       </c>
@@ -739,7 +704,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>36</v>
       </c>
@@ -759,7 +724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>111</v>
       </c>
@@ -779,7 +744,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>87</v>
       </c>
@@ -799,7 +764,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>203</v>
       </c>
@@ -819,7 +784,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>140</v>
       </c>

</xml_diff>